<commit_message>
cut rrp break points
</commit_message>
<xml_diff>
--- a/users/XiaodanLyu/feature_engineering/fct_relabel.xlsx
+++ b/users/XiaodanLyu/feature_engineering/fct_relabel.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="color" sheetId="1" r:id="rId1"/>
     <sheet name="brand" sheetId="2" r:id="rId2"/>
     <sheet name="size" sheetId="4" r:id="rId3"/>
-    <sheet name="brand_survey" sheetId="3" r:id="rId4"/>
-    <sheet name="brand_others" sheetId="5" r:id="rId5"/>
+    <sheet name="cut" sheetId="6" r:id="rId4"/>
+    <sheet name="brand_survey" sheetId="3" r:id="rId5"/>
+    <sheet name="brand_others" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="277">
   <si>
     <t>old_levels</t>
   </si>
@@ -866,6 +867,27 @@
   <si>
     <t>brand.competition</t>
     <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>cut.reason</t>
+  </si>
+  <si>
+    <t>cut.break</t>
+  </si>
+  <si>
+    <t>rrp</t>
+  </si>
+  <si>
+    <t>cat1</t>
+  </si>
+  <si>
+    <t>cat2</t>
+  </si>
+  <si>
+    <t>cat3</t>
   </si>
 </sst>
 </file>
@@ -3044,7 +3066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -6643,6 +6665,92 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -6820,7 +6928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>

</xml_diff>